<commit_message>
update report with bug/flaw findings
</commit_message>
<xml_diff>
--- a/Downloads/DefectReport.xlsx
+++ b/Downloads/DefectReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>Defect ID</t>
   </si>
@@ -33,13 +33,241 @@
     <t>Test Steps</t>
   </si>
   <si>
-    <t>API delete request is not working as it returns an unauthorized use code</t>
-  </si>
-  <si>
-    <t>API response should return a code of 200. When a get employee list is sent, the deleted employee should not be in response.</t>
-  </si>
-  <si>
-    <t>API delete response returned an unauthorized code. A subsequent employee list get still returns the employee in the response.</t>
+    <t xml:space="preserve">On the dashboard, the employees' last names are in the first name column and the first names are in the last name column. </t>
+  </si>
+  <si>
+    <t>The first and last names for each employee should be under their respective column accordingly.</t>
+  </si>
+  <si>
+    <t>Last name data is under First Name column and first name data is under Last Name column.</t>
+  </si>
+  <si>
+    <t>When editing an existing employee, the popup window to allow data input has the "Dependents" title misspelled as "Dependants."</t>
+  </si>
+  <si>
+    <t>During an Edit operation all input labels should have the correct spelling.</t>
+  </si>
+  <si>
+    <t>The "Dependents" label in the popup window is spelled as "Dependants."</t>
+  </si>
+  <si>
+    <t>The edit popup window is incorreclty titled as "Add Employee".</t>
+  </si>
+  <si>
+    <t>During an Edit operation the window title should be "Edit Employee."</t>
+  </si>
+  <si>
+    <t>The title for the Edit Employee window is Add Employee.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dashboard should display dollar entries (amounts) as such. </t>
+  </si>
+  <si>
+    <t>The dashboard should show data specifying dollar amounts such as "Salary" and "Benefit Cost" with "$."</t>
+  </si>
+  <si>
+    <t>The dashboard shows data without dollar amount indication "$."</t>
+  </si>
+  <si>
+    <t>After selecting the Delete icon from the dashboard for an employee and clicking the Delete button on the popup window, the delete operation should complete and close the delete popup window.</t>
+  </si>
+  <si>
+    <t>In the delete operation when the Delete button is clicked, a verification step should be provided to allow employer second chance to cancel delete operation.</t>
+  </si>
+  <si>
+    <t>When the Delete button is clicked on the delete popup window, the employer should be askd a second time if the data should be deleted to make sure the employer does want to delete the employee.</t>
+  </si>
+  <si>
+    <t>When the Delete button is clicked on the delete popup window, the employer  is not given an opportunity to cancel the delete operation.</t>
+  </si>
+  <si>
+    <t>After changing the first name or last name in the edit operation, clicking the Update button should complete the operation and close the edit popup window.</t>
+  </si>
+  <si>
+    <t>In the edit operation, entering nonalphabetic haracters for the first name or last name is not addressed in the input</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is not alphabetic and even special characters, an error message should be provided and the employer should have to reenter it.</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is not alphabetic, such as "&gt;?.," the edit operation completes after clicking the Update button and the erroroneous name is seen in the dashboard.</t>
+  </si>
+  <si>
+    <t>There should be a range provided for the number of eligible depedents so the employer can provide a value within range.</t>
+  </si>
+  <si>
+    <t>If the employer provides a number out of range, clicking the Update button does not allow the edit operation to complete and the popup window sits there. It appears the range is 0-32.</t>
+  </si>
+  <si>
+    <t>After changing the first name or last name in the edit operation, clicking the Update button does not provide an edit completion. The edit popup window remains visible. However, this did work at other times so an investigation is required.</t>
+  </si>
+  <si>
+    <t>In the edit operation, the input for the number of dependents should specify a maximum number.</t>
+  </si>
+  <si>
+    <t>In the edit operation, the employer can leave the number of dependents field empty and update it.</t>
+  </si>
+  <si>
+    <t>The employer should not be able to leave the number of dependents empty and complete the edit operation. This should be a non-null field and an input should be required.</t>
+  </si>
+  <si>
+    <t>The employer can leave the number of dependents field without an input and complete the Update operation. In the dashboard, the number of dependents does indicate zero.</t>
+  </si>
+  <si>
+    <t>In the delete operation, the delete operation does not complete. This appears to be an intermittent issue.</t>
+  </si>
+  <si>
+    <t>After selecting the Delete icon from the dashboard for an employee and clicking the Delete button on the popup window, the delete operation does not complete and the delete popup window remains open. This appears to be intermittent since I was able to complete the deletion at other times. This needs to be investigated.</t>
+  </si>
+  <si>
+    <t>In the add employee operation, entering nonalphabetic haracters for the first name or last name is not addressed in the input</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is not alphabetic, such as "&gt;?.," the add operation completes after clicking the Add button and the erroroneous name is seen in the dashboard.</t>
+  </si>
+  <si>
+    <t>In the add employee operation, the input for the number of dependents should specify a maximum number.</t>
+  </si>
+  <si>
+    <t>If the employer provides a number out of range, clicking the Add button does not allow the add operation to complete and the popup window sits there. It looks like the range is 0-32.</t>
+  </si>
+  <si>
+    <t>In the add employee operation, the employer can leave the number of dependents field empty and update it.</t>
+  </si>
+  <si>
+    <t>The employer should not be able to leave the number of dependents empty and complete the add operation. This should be a non-null field and an input should be required.</t>
+  </si>
+  <si>
+    <t>The employer can leave the number of dependents field without an input and complete the Add operation. In the dashboard, the number of dependents does indicate zero.</t>
+  </si>
+  <si>
+    <t>The employer should not be able to add another employee entry with the same first name, last name, and number of dependents after successfully adding the first entry. The add operation should not allow this and provide an error message.</t>
+  </si>
+  <si>
+    <t>The employer added an employee in the add operation. After reviewing in the dashboard, the employer adds another employee entry with the same first name, last name, and number of dependents. The add operation completed and two similar entries with different IDs are seen on the dashboard.</t>
+  </si>
+  <si>
+    <t>When adding a new employee, the popup window to allow data input has the "Dependents" label misspelled as "Dependants."</t>
+  </si>
+  <si>
+    <t>During an Add operation all input labels should have the correct spelling.</t>
+  </si>
+  <si>
+    <t>The "Dependents" label in the popup window is spelled as "Dependants" for the add operation when adding a new employee entry.</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is not entered and left blank, an error message should be provided to specify that the field must be populated.</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is not entered and left blank, the employer is not given an error message and can continue the input of other fields.</t>
+  </si>
+  <si>
+    <t>In the edit operation, blanking out  a first name or last name should provide an error message indicating it must be input.</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is removed and left blank, an error message should be provided to specify that the field must be populated.</t>
+  </si>
+  <si>
+    <t>When the input to the first name or last name is removed and left blank, the employer is not given an error message and can continue the input of other fields.</t>
+  </si>
+  <si>
+    <t>In the add operation, not entering a first name or last name should provide an error message indicating it must be input.</t>
+  </si>
+  <si>
+    <t>In API testing using Postman, the Get Employee request requires the basic authorization with username and password rather than the basic token as described in the Postman documentation.</t>
+  </si>
+  <si>
+    <t>The authorization token should be included in the GET employee request in the authorization part of the header to allow the request to provide a response and complete.</t>
+  </si>
+  <si>
+    <t>Using the authorization token returned an unauthorized response code 401 instead of 200.</t>
+  </si>
+  <si>
+    <t>In API testing using Postman, the Put Employee request allows the changing of the first name and last name to non-alphabetic characters.</t>
+  </si>
+  <si>
+    <t>The PUT Employee request should not be allowed to update and an error response should be provided indicating the type of error made.</t>
+  </si>
+  <si>
+    <t>The PUT Employee request has non-alphabetic characters, such as "?&gt;,,," for the first or last name and is sent. The update is made with a response code of 200. The dashboard displays the badly-formed name.</t>
+  </si>
+  <si>
+    <t>In API testing using Postman, the DEL Employee request to delete an employee has a non-existing employee id sent. The reponse message should indicate that no deletion was made.</t>
+  </si>
+  <si>
+    <t>The DEL Employee request should have a response code other than 200 and a message indicating that the employee ID does not exist so no deletion was made.</t>
+  </si>
+  <si>
+    <t>The DEL Employee request returned a response code of 200 so employer does not realize a non-existing ID was populated in the request.</t>
+  </si>
+  <si>
+    <t>In API testing using Postman, the Get Employee request is sent with a non-existing employee ID and the response code is 200.</t>
+  </si>
+  <si>
+    <t>The GET Employee with a bad employee ID should return a response code other than 200 (OK) even though there is no message body.</t>
+  </si>
+  <si>
+    <t>The GET Employee request with a bad Employee ID returns a response code of 200 indicating that the request did not encounter any errors.</t>
+  </si>
+  <si>
+    <t>On the dashboard view, the Paylocity Dashboard Benefits title is clickable but it just causes a refresh of the current view.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Paylocity Dashboard Benefits title should not be clickable when moused over. </t>
+  </si>
+  <si>
+    <t>Mousing over the title allows the Employer to refresh the current view. This can be done also on the refresh on the browser panel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PUT Employee request is sent with a valid, updated dependent value and a response code of 200 is returned. However, the number of dependent value is updated to zero in the message response body. As a result, the other values such as net, benefits cost, etc. are updated according to no dependents. </t>
+  </si>
+  <si>
+    <t>In API testing using Postman, the POST Employee request can be sent twice with the same input data which adds duplicate emploee entries.</t>
+  </si>
+  <si>
+    <t>Two POST Employee request with the exact same data should not allow duplicate entries to be created in the database. The second POST Employee request should not complete and return with a code indicating that the add did not complete.</t>
+  </si>
+  <si>
+    <t>The first POST Employee request returned a response message with code 200 and the message body displayed relevant data. The second POST Employee request also returned a 200 message response with a completed message body. Both entries can be seen on the dashboard.</t>
+  </si>
+  <si>
+    <t>In the edit operation after changing the first or last name, the edit operation does not complete. This appears to be intermittent.</t>
+  </si>
+  <si>
+    <t>The PUT Employee request should be allowed to change the number of dependents and the response should display the updated value with a response code of 200. The values affected by the dependents should be updated appropriately.</t>
+  </si>
+  <si>
+    <t>1. Use a PUT Employee message format and specify the authorization code as the basic token and the content type to be JSON in the message header.                                                                     2. In the message body, provide the ID of an existing employee entry and the same first name and last name values. Use the GET Employee List to find one.                                                                 3. For the number of dependents, use a different value from the existing value.                                                                                              4. Click on the Send button in Postman.                                                    5. The response message has a code of 200 (OK).                                6. The message body should have the previous employee ID, first name, and last name. The number of dependents has a value of zero instead of the new value. The benefits cost and net has values of 38.46154 and 1961.53845, respectively.                 7. Also verify these new values on the benefits dashboard.</t>
+  </si>
+  <si>
+    <t>When the Employer logs into the Paylocity Benefits Dashboard, the list of present employees should be ordered in a logical manner, such as the employee last name, so that a particular employee may be found easily since there are a large number of employees.</t>
+  </si>
+  <si>
+    <t>The dashboard has the existing employee information ordered by employee ID. It would be difficult to quickly access a specific employee in such a manner.</t>
+  </si>
+  <si>
+    <t>The Paylocity Benefits Dashboard does not create pages for the Employer to traverse when there are a large number of employee entries, more than 30.</t>
+  </si>
+  <si>
+    <t>When the Employer logs into the Paylocity Benefits Dashboard, the list of present employees should be listed on pages, such as 10-15 per page, in order for the Employer to access a particular employee faster.</t>
+  </si>
+  <si>
+    <t>The dashboard has the existing employee information on one page so the Employer would need to use the vertical scroll bar to move through the information and locate the employee data being sought.</t>
+  </si>
+  <si>
+    <t>In the add employee operation, duplicate entries can be added with similar data.</t>
+  </si>
+  <si>
+    <t>1. The Employer logs into the Paylocaity Benefits Dashboard site using username and password. The dashboard is displayed with the current employee records.                                                                    2. The Employer selects an existing employee entry and clicks on the edit/update operation under the Actions column.               3. An edit popup window is displayed with the current first name, last name, and number of dependents.                                     4. Move the focus to the last name editbox and change the value with special characters, "?&gt;&gt;,,."                                                       5. Click on the Update button to complete the edit operation and the popup window closes.                                                                    6. Verify that the last name has been changed to "?&gt;&gt;,,." on the dashboard.</t>
+  </si>
+  <si>
+    <t>1. The Employer logs into the Paylocaity Benefits Dashboard site using username and password. The dashboard is displayed with the current employee records.                                                                    2. The Employer clicks on the Add Employee button at the page bottom. A popup window to add an employee appears.                  3. Enter "Tom" for the First Name, "Smith" for the Last Name, and "3" for Dependants. Then click on the Add button.                    4. The add operation completes and an entry with the added data is seen on the dashboard.                                                                     5. Again, the Employer clicks on the Add Employee button at the page bottom. A popup window to add an employee appears.                                                                                                                6. Again, enter "Tom" for the First Name, "Smith" for the Last Name, and "3" for Dependants. Then click on the Add button.     7. The second add operation completes and an entry with the added data can be found on the dashboard.                                          8. Verify that there are two employee records with "Tom" as the first name, "Smith" as the last name, and Dependents as "3." The only difference is the employee ID between the two entries.</t>
+  </si>
+  <si>
+    <t>The list of employees in the Paylocity Benefits Dashboard are ordered by Employee ID which is not very intuitive. Should be ordered by employee last name instead or better yet, click on a column heading and order the data by the column data.</t>
+  </si>
+  <si>
+    <t>In API testing using Postman, the Put Employee request is used to change the number of dependents but it updates to zero dependents and the update completes.</t>
   </si>
 </sst>
 </file>
@@ -69,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -92,11 +320,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -108,6 +347,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,10 +666,10 @@
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +685,15 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -455,9 +707,573 @@
         <v>7</v>
       </c>
       <c r="E2" s="3"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+    </row>
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="1:12" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:12" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="1:12" s="4" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="1:12" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="1:12" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>